<commit_message>
or_algorithm Klasse algorithmus in Methoden
</commit_message>
<xml_diff>
--- a/Einsatzplan.xlsx
+++ b/Einsatzplan.xlsx
@@ -41,14 +41,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
-        <bgColor rgb="0000FF00"/>
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1115,156 +1115,156 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1005</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="V2" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="X2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="AC2" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD2" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AG2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="AO2" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AZ2" s="4" t="n"/>
@@ -1330,156 +1330,156 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1007</v>
-      </c>
-      <c r="B3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3" t="n">
         <v>0</v>
       </c>
       <c r="V3" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AF3" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AN3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AZ3" s="4" t="n"/>
@@ -1545,157 +1545,157 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1008</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="R4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="T4" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AD4" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AX4" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY4" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ4" s="4" t="n"/>
       <c r="BA4" s="4" t="n"/>
@@ -1760,156 +1760,156 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1009</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="W5" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AC5" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="AH5" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AQ5" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AZ5" s="4" t="n"/>
@@ -1975,157 +1975,157 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1004</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="T6" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AH6" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI6" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="AX6" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY6" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ6" s="4" t="n"/>
       <c r="BA6" s="4" t="n"/>

</xml_diff>

<commit_message>
some changes for server
</commit_message>
<xml_diff>
--- a/Einsatzplan.xlsx
+++ b/Einsatzplan.xlsx
@@ -2239,8 +2239,8 @@
       <c r="S2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="T2" s="2" t="n">
-        <v>1</v>
+      <c r="T2" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="U2" s="3" t="n">
         <v>0</v>
@@ -2283,62 +2283,62 @@
           <t> </t>
         </is>
       </c>
-      <c r="AH2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ2" s="2" t="n">
-        <v>1</v>
+      <c r="AH2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="BA2" s="3" t="n">
         <v>0</v>
@@ -2479,62 +2479,62 @@
           <t> </t>
         </is>
       </c>
-      <c r="CT2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CX2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CY2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CZ2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DA2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DB2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DC2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DD2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DE2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DF2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DG2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DH2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DI2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DJ2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DK2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DL2" s="3" t="n">
-        <v>0</v>
+      <c r="CT2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CU2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CV2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CW2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CX2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CY2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CZ2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DA2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DB2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DC2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DD2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DE2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DF2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DG2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DH2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DI2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DJ2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DK2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DL2" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="DM2" s="3" t="n">
         <v>0</v>
@@ -2846,8 +2846,8 @@
       <c r="J3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="2" t="n">
-        <v>1</v>
+      <c r="K3" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="L3" s="2" t="n">
         <v>1</v>
@@ -2894,11 +2894,11 @@
       <c r="Z3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="AA3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="2" t="n">
-        <v>1</v>
+      <c r="AA3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="AC3" s="3" t="n">
         <v>0</v>
@@ -2947,32 +2947,32 @@
       <c r="AQ3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="AR3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ3" s="3" t="n">
-        <v>0</v>
+      <c r="AR3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ3" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="BA3" s="2" t="n">
         <v>1</v>
@@ -2992,11 +2992,11 @@
       <c r="BF3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="BG3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="BH3" s="2" t="n">
-        <v>1</v>
+      <c r="BG3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH3" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="BI3" s="3" t="n">
         <v>0</v>
@@ -3060,17 +3060,17 @@
       <c r="CB3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="CC3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CD3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CE3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CF3" s="2" t="n">
-        <v>1</v>
+      <c r="CC3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF3" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="CG3" s="2" t="n">
         <v>1</v>
@@ -3140,44 +3140,44 @@
       <c r="DB3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="DC3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DD3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DE3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DF3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DG3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DH3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DI3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DJ3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DK3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DL3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DM3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DN3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DO3" s="2" t="n">
-        <v>1</v>
+      <c r="DC3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DD3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DE3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DF3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DG3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DH3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO3" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="DP3" s="3" t="n">
         <v>0</v>
@@ -3253,44 +3253,44 @@
       <c r="EM3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="EN3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EO3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EP3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EQ3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="ER3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="ES3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="ET3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EU3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EV3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EW3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EY3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EZ3" s="3" t="n">
-        <v>0</v>
+      <c r="EN3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EO3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EP3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EQ3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="ER3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="ES3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="ET3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EU3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EV3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EW3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EX3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EY3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EZ3" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="FA3" s="3" t="n">
         <v>0</v>
@@ -3507,8 +3507,8 @@
       <c r="S4" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="T4" s="3" t="n">
-        <v>0</v>
+      <c r="T4" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="U4" s="2" t="n">
         <v>1</v>
@@ -3715,32 +3715,32 @@
       <c r="CI4" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="CJ4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR4" s="3" t="n">
-        <v>0</v>
+      <c r="CJ4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CK4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CL4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CM4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CN4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CO4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CP4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CQ4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CR4" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="CS4" s="4" t="inlineStr">
         <is>
@@ -3911,32 +3911,32 @@
       <c r="EU4" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="EV4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EW4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EX4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EY4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EZ4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="FA4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="FB4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="FC4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="FD4" s="2" t="n">
-        <v>1</v>
+      <c r="EV4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EW4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EY4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EZ4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="FA4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="FB4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="FC4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="FD4" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="FE4" s="4" t="inlineStr">
         <is>
@@ -4301,17 +4301,17 @@
       <c r="BS5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="BT5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="BU5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="BV5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="BW5" s="2" t="n">
-        <v>1</v>
+      <c r="BT5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BU5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BW5" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="BX5" s="2" t="n">
         <v>1</v>
@@ -4328,11 +4328,11 @@
       <c r="CB5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="CC5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CD5" s="3" t="n">
-        <v>0</v>
+      <c r="CC5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD5" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="CE5" s="3" t="n">
         <v>0</v>
@@ -4381,20 +4381,20 @@
           <t> </t>
         </is>
       </c>
-      <c r="CT5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CX5" s="3" t="n">
-        <v>0</v>
+      <c r="CT5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CU5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CV5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CW5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CX5" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="CY5" s="2" t="n">
         <v>1</v>
@@ -4435,8 +4435,8 @@
       <c r="DK5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="DL5" s="2" t="n">
-        <v>1</v>
+      <c r="DL5" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="DM5" s="3" t="n">
         <v>0</v>
@@ -4494,8 +4494,8 @@
       <c r="ED5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="EE5" s="3" t="n">
-        <v>0</v>
+      <c r="EE5" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="EF5" s="2" t="n">
         <v>1</v>
@@ -4521,14 +4521,14 @@
       <c r="EM5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="EN5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EO5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EP5" s="2" t="n">
-        <v>1</v>
+      <c r="EN5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EO5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EP5" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="EQ5" s="3" t="n">
         <v>0</v>
@@ -4748,8 +4748,8 @@
       <c r="J6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="3" t="n">
-        <v>0</v>
+      <c r="K6" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="L6" s="3" t="n">
         <v>0</v>
@@ -4819,35 +4819,35 @@
           <t> </t>
         </is>
       </c>
-      <c r="AH6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="3" t="n">
-        <v>0</v>
+      <c r="AH6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="AR6" s="3" t="n">
         <v>0</v>
@@ -4935,17 +4935,17 @@
       <c r="BS6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="BT6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BV6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BW6" s="3" t="n">
-        <v>0</v>
+      <c r="BT6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BU6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW6" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="BX6" s="3" t="n">
         <v>0</v>
@@ -5015,32 +5015,32 @@
           <t> </t>
         </is>
       </c>
-      <c r="CT6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CU6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CV6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CW6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CX6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CY6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CZ6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DA6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DB6" s="2" t="n">
-        <v>1</v>
+      <c r="CT6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CY6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CZ6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DA6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DB6" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="DC6" s="3" t="n">
         <v>0</v>
@@ -5113,23 +5113,23 @@
           <t> </t>
         </is>
       </c>
-      <c r="DZ6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EA6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EB6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EC6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="ED6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EE6" s="2" t="n">
-        <v>1</v>
+      <c r="DZ6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EA6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EB6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EC6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EE6" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="EF6" s="3" t="n">
         <v>0</v>
@@ -5608,29 +5608,29 @@
       <c r="CF7" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="CG7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CH7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CI7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CJ7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CK7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CL7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CM7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CN7" s="2" t="n">
-        <v>1</v>
+      <c r="CG7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN7" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="CO7" s="2" t="n">
         <v>1</v>
@@ -5724,23 +5724,23 @@
       <c r="DR7" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="DS7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DT7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DU7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DV7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DW7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DX7" s="3" t="n">
-        <v>0</v>
+      <c r="DS7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DT7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DU7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DV7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DW7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DX7" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="DY7" s="4" t="inlineStr">
         <is>
@@ -6064,23 +6064,23 @@
       <c r="Z8" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="AA8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="3" t="n">
-        <v>0</v>
+      <c r="AA8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="AG8" s="4" t="inlineStr">
         <is>
@@ -6168,17 +6168,17 @@
       <c r="BH8" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="BI8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="BJ8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="BK8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL8" s="2" t="n">
-        <v>1</v>
+      <c r="BI8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="BM8" s="4" t="inlineStr">
         <is>
@@ -6456,11 +6456,11 @@
       <c r="EX8" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="EY8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EZ8" s="2" t="n">
-        <v>1</v>
+      <c r="EY8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EZ8" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="FA8" s="2" t="n">
         <v>1</v>
@@ -7338,17 +7338,17 @@
       <c r="AB10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="AC10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="2" t="n">
-        <v>1</v>
+      <c r="AC10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="AG10" s="4" t="inlineStr">
         <is>
@@ -7430,23 +7430,23 @@
       <c r="BF10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="BG10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BJ10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BK10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL10" s="3" t="n">
-        <v>0</v>
+      <c r="BG10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL10" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="BM10" s="4" t="inlineStr">
         <is>
@@ -7504,20 +7504,20 @@
       <c r="CD10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="CE10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI10" s="3" t="n">
-        <v>0</v>
+      <c r="CE10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CG10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CI10" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="CJ10" s="3" t="n">
         <v>0</v>
@@ -7534,17 +7534,17 @@
       <c r="CN10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="CO10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CP10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CQ10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CR10" s="2" t="n">
-        <v>1</v>
+      <c r="CO10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR10" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="CS10" s="4" t="inlineStr">
         <is>
@@ -7605,17 +7605,17 @@
       <c r="DK10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="DL10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DM10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DN10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DO10" s="3" t="n">
-        <v>0</v>
+      <c r="DL10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DM10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO10" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="DP10" s="3" t="n">
         <v>0</v>
@@ -7626,23 +7626,23 @@
       <c r="DR10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="DS10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DT10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DU10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DV10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DW10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DX10" s="2" t="n">
-        <v>1</v>
+      <c r="DS10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DU10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DV10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DW10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DX10" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="DY10" s="4" t="inlineStr">
         <is>
@@ -7700,20 +7700,20 @@
       <c r="EP10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="EQ10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="ER10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="ES10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="ET10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="EU10" s="2" t="n">
-        <v>1</v>
+      <c r="EQ10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="ER10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="ES10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="ET10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="EU10" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="EV10" s="3" t="n">
         <v>0</v>
@@ -7724,23 +7724,23 @@
       <c r="EX10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="EY10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EZ10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="FA10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="FB10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="FC10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="FD10" s="3" t="n">
-        <v>0</v>
+      <c r="EY10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EZ10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="FA10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="FB10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="FC10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="FD10" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="FE10" s="4" t="inlineStr">
         <is>
@@ -8185,20 +8185,20 @@
           <t> </t>
         </is>
       </c>
-      <c r="CT11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CU11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CV11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CW11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CX11" s="2" t="n">
-        <v>1</v>
+      <c r="CT11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX11" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="CY11" s="3" t="n">
         <v>0</v>
@@ -8283,20 +8283,20 @@
           <t> </t>
         </is>
       </c>
-      <c r="DZ11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EA11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EB11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EC11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="ED11" s="3" t="n">
-        <v>0</v>
+      <c r="DZ11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EA11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EB11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="EC11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="ED11" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="EE11" s="3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Skills in NBs eingebaut
</commit_message>
<xml_diff>
--- a/Einsatzplan.xlsx
+++ b/Einsatzplan.xlsx
@@ -790,22 +790,86 @@
           <t> </t>
         </is>
       </c>
-      <c r="G3" s="2" t="n"/>
-      <c r="H3" s="2" t="n"/>
-      <c r="I3" s="2" t="n"/>
-      <c r="J3" s="2" t="n"/>
-      <c r="K3" s="2" t="n"/>
-      <c r="L3" s="2" t="n"/>
-      <c r="M3" s="2" t="n"/>
-      <c r="N3" s="2" t="n"/>
-      <c r="O3" s="2" t="n"/>
-      <c r="P3" s="2" t="n"/>
-      <c r="Q3" s="2" t="n"/>
-      <c r="R3" s="2" t="n"/>
-      <c r="S3" s="2" t="n"/>
-      <c r="T3" s="2" t="n"/>
-      <c r="U3" s="2" t="n"/>
-      <c r="V3" s="2" t="n"/>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="O3" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="Q3" s="2" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="R3" s="2" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="S3" s="2" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="U3" s="2" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="W3" s="2" t="n"/>
       <c r="X3" s="2" t="n"/>
       <c r="Y3" s="2" t="n"/>

</xml_diff>

<commit_message>
Skill bei a eingebaut, evtl. a[i,j] implementieren
</commit_message>
<xml_diff>
--- a/Einsatzplan.xlsx
+++ b/Einsatzplan.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CF3"/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,47 +472,6 @@
     <col width="3" customWidth="1" min="41" max="41"/>
     <col width="3" customWidth="1" min="42" max="42"/>
     <col width="3" customWidth="1" min="43" max="43"/>
-    <col width="3" customWidth="1" min="44" max="44"/>
-    <col width="3" customWidth="1" min="45" max="45"/>
-    <col width="3" customWidth="1" min="46" max="46"/>
-    <col width="3" customWidth="1" min="47" max="47"/>
-    <col width="3" customWidth="1" min="48" max="48"/>
-    <col width="3" customWidth="1" min="49" max="49"/>
-    <col width="3" customWidth="1" min="50" max="50"/>
-    <col width="3" customWidth="1" min="51" max="51"/>
-    <col width="3" customWidth="1" min="52" max="52"/>
-    <col width="3" customWidth="1" min="53" max="53"/>
-    <col width="3" customWidth="1" min="54" max="54"/>
-    <col width="3" customWidth="1" min="55" max="55"/>
-    <col width="3" customWidth="1" min="56" max="56"/>
-    <col width="3" customWidth="1" min="57" max="57"/>
-    <col width="3" customWidth="1" min="58" max="58"/>
-    <col width="3" customWidth="1" min="59" max="59"/>
-    <col width="3" customWidth="1" min="60" max="60"/>
-    <col width="3" customWidth="1" min="61" max="61"/>
-    <col width="3" customWidth="1" min="62" max="62"/>
-    <col width="3" customWidth="1" min="63" max="63"/>
-    <col width="3" customWidth="1" min="64" max="64"/>
-    <col width="3" customWidth="1" min="65" max="65"/>
-    <col width="3" customWidth="1" min="66" max="66"/>
-    <col width="3" customWidth="1" min="67" max="67"/>
-    <col width="3" customWidth="1" min="68" max="68"/>
-    <col width="3" customWidth="1" min="69" max="69"/>
-    <col width="3" customWidth="1" min="70" max="70"/>
-    <col width="3" customWidth="1" min="71" max="71"/>
-    <col width="3" customWidth="1" min="72" max="72"/>
-    <col width="3" customWidth="1" min="73" max="73"/>
-    <col width="3" customWidth="1" min="74" max="74"/>
-    <col width="3" customWidth="1" min="75" max="75"/>
-    <col width="3" customWidth="1" min="76" max="76"/>
-    <col width="3" customWidth="1" min="77" max="77"/>
-    <col width="3" customWidth="1" min="78" max="78"/>
-    <col width="3" customWidth="1" min="79" max="79"/>
-    <col width="3" customWidth="1" min="80" max="80"/>
-    <col width="3" customWidth="1" min="81" max="81"/>
-    <col width="3" customWidth="1" min="82" max="82"/>
-    <col width="3" customWidth="1" min="83" max="83"/>
-    <col width="3" customWidth="1" min="84" max="84"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -728,218 +687,13 @@
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>T2, 8:0</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 8:15</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 8:30</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 8:45</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 9:0</t>
-        </is>
-      </c>
-      <c r="AV1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 9:15</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 9:30</t>
-        </is>
-      </c>
-      <c r="AX1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 9:45</t>
-        </is>
-      </c>
-      <c r="AY1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 10:0</t>
-        </is>
-      </c>
-      <c r="AZ1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 10:15</t>
-        </is>
-      </c>
-      <c r="BA1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 10:30</t>
-        </is>
-      </c>
-      <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 10:45</t>
-        </is>
-      </c>
-      <c r="BC1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 11:0</t>
-        </is>
-      </c>
-      <c r="BD1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 11:15</t>
-        </is>
-      </c>
-      <c r="BE1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 11:30</t>
-        </is>
-      </c>
-      <c r="BF1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 11:45</t>
-        </is>
-      </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 12:0</t>
-        </is>
-      </c>
-      <c r="BH1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 12:15</t>
-        </is>
-      </c>
-      <c r="BI1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 12:30</t>
-        </is>
-      </c>
-      <c r="BJ1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 12:45</t>
-        </is>
-      </c>
-      <c r="BK1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 13:0</t>
-        </is>
-      </c>
-      <c r="BL1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 13:15</t>
-        </is>
-      </c>
-      <c r="BM1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 13:30</t>
-        </is>
-      </c>
-      <c r="BN1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 13:45</t>
-        </is>
-      </c>
-      <c r="BO1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 14:0</t>
-        </is>
-      </c>
-      <c r="BP1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 14:15</t>
-        </is>
-      </c>
-      <c r="BQ1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 14:30</t>
-        </is>
-      </c>
-      <c r="BR1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 14:45</t>
-        </is>
-      </c>
-      <c r="BS1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 15:0</t>
-        </is>
-      </c>
-      <c r="BT1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 15:15</t>
-        </is>
-      </c>
-      <c r="BU1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 15:30</t>
-        </is>
-      </c>
-      <c r="BV1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 15:45</t>
-        </is>
-      </c>
-      <c r="BW1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 16:0</t>
-        </is>
-      </c>
-      <c r="BX1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 16:15</t>
-        </is>
-      </c>
-      <c r="BY1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 16:30</t>
-        </is>
-      </c>
-      <c r="BZ1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 16:45</t>
-        </is>
-      </c>
-      <c r="CA1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 17:0</t>
-        </is>
-      </c>
-      <c r="CB1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 17:15</t>
-        </is>
-      </c>
-      <c r="CC1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 17:30</t>
-        </is>
-      </c>
-      <c r="CD1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 17:45</t>
-        </is>
-      </c>
-      <c r="CE1" s="1" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="CF1" s="1" t="inlineStr">
-        <is>
           <t>Total Hours</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
@@ -966,86 +720,22 @@
           <t> </t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>v</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>i</t>
-        </is>
-      </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
-        <is>
-          <t>p</t>
-        </is>
-      </c>
-      <c r="O2" s="2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="P2" s="2" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="Q2" s="2" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="R2" s="2" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="S2" s="2" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="T2" s="2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="U2" s="2" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-      <c r="V2" s="2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
+      <c r="M2" s="2" t="n"/>
+      <c r="N2" s="2" t="n"/>
+      <c r="O2" s="2" t="n"/>
+      <c r="P2" s="2" t="n"/>
+      <c r="Q2" s="2" t="n"/>
+      <c r="R2" s="2" t="n"/>
+      <c r="S2" s="2" t="n"/>
+      <c r="T2" s="2" t="n"/>
+      <c r="U2" s="2" t="n"/>
+      <c r="V2" s="2" t="n"/>
       <c r="W2" s="2" t="n"/>
       <c r="X2" s="2" t="n"/>
       <c r="Y2" s="2" t="n"/>
@@ -1066,55 +756,14 @@
       <c r="AN2" s="2" t="n"/>
       <c r="AO2" s="2" t="n"/>
       <c r="AP2" s="2" t="n"/>
-      <c r="AQ2" s="2" t="n"/>
-      <c r="AR2" s="2" t="n"/>
-      <c r="AS2" s="2" t="n"/>
-      <c r="AT2" s="2" t="n"/>
-      <c r="AU2" s="2" t="n"/>
-      <c r="AV2" s="2" t="n"/>
-      <c r="AW2" s="2" t="n"/>
-      <c r="AX2" s="2" t="n"/>
-      <c r="AY2" s="2" t="n"/>
-      <c r="AZ2" s="2" t="n"/>
-      <c r="BA2" s="2" t="n"/>
-      <c r="BB2" s="2" t="n"/>
-      <c r="BC2" s="2" t="n"/>
-      <c r="BD2" s="2" t="n"/>
-      <c r="BE2" s="2" t="n"/>
-      <c r="BF2" s="2" t="n"/>
-      <c r="BG2" s="2" t="n"/>
-      <c r="BH2" s="2" t="n"/>
-      <c r="BI2" s="2" t="n"/>
-      <c r="BJ2" s="2" t="n"/>
-      <c r="BK2" s="2" t="n"/>
-      <c r="BL2" s="2" t="n"/>
-      <c r="BM2" s="2" t="n"/>
-      <c r="BN2" s="2" t="n"/>
-      <c r="BO2" s="2" t="n"/>
-      <c r="BP2" s="2" t="n"/>
-      <c r="BQ2" s="2" t="n"/>
-      <c r="BR2" s="2" t="n"/>
-      <c r="BS2" s="2" t="n"/>
-      <c r="BT2" s="2" t="n"/>
-      <c r="BU2" s="2" t="n"/>
-      <c r="BV2" s="2" t="n"/>
-      <c r="BW2" s="2" t="n"/>
-      <c r="BX2" s="2" t="n"/>
-      <c r="BY2" s="2" t="n"/>
-      <c r="BZ2" s="2" t="n"/>
-      <c r="CA2" s="2" t="n"/>
-      <c r="CB2" s="2" t="n"/>
-      <c r="CC2" s="2" t="n"/>
-      <c r="CD2" s="2" t="n"/>
-      <c r="CE2" s="2" t="n"/>
-      <c r="CF2" s="2">
-        <f>SUM(B2:CE2)</f>
+      <c r="AQ2" s="2">
+        <f>SUM(B2:AP2)</f>
         <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
@@ -1141,22 +790,86 @@
           <t> </t>
         </is>
       </c>
-      <c r="G3" s="2" t="n"/>
-      <c r="H3" s="2" t="n"/>
-      <c r="I3" s="2" t="n"/>
-      <c r="J3" s="2" t="n"/>
-      <c r="K3" s="2" t="n"/>
-      <c r="L3" s="2" t="n"/>
-      <c r="M3" s="2" t="n"/>
-      <c r="N3" s="2" t="n"/>
-      <c r="O3" s="2" t="n"/>
-      <c r="P3" s="2" t="n"/>
-      <c r="Q3" s="2" t="n"/>
-      <c r="R3" s="2" t="n"/>
-      <c r="S3" s="2" t="n"/>
-      <c r="T3" s="2" t="n"/>
-      <c r="U3" s="2" t="n"/>
-      <c r="V3" s="2" t="n"/>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="O3" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="Q3" s="2" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="R3" s="2" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="S3" s="2" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="U3" s="2" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="W3" s="2" t="n"/>
       <c r="X3" s="2" t="n"/>
       <c r="Y3" s="2" t="n"/>
@@ -1177,49 +890,8 @@
       <c r="AN3" s="2" t="n"/>
       <c r="AO3" s="2" t="n"/>
       <c r="AP3" s="2" t="n"/>
-      <c r="AQ3" s="2" t="n"/>
-      <c r="AR3" s="2" t="n"/>
-      <c r="AS3" s="2" t="n"/>
-      <c r="AT3" s="2" t="n"/>
-      <c r="AU3" s="2" t="n"/>
-      <c r="AV3" s="2" t="n"/>
-      <c r="AW3" s="2" t="n"/>
-      <c r="AX3" s="2" t="n"/>
-      <c r="AY3" s="2" t="n"/>
-      <c r="AZ3" s="2" t="n"/>
-      <c r="BA3" s="2" t="n"/>
-      <c r="BB3" s="2" t="n"/>
-      <c r="BC3" s="2" t="n"/>
-      <c r="BD3" s="2" t="n"/>
-      <c r="BE3" s="2" t="n"/>
-      <c r="BF3" s="2" t="n"/>
-      <c r="BG3" s="2" t="n"/>
-      <c r="BH3" s="2" t="n"/>
-      <c r="BI3" s="2" t="n"/>
-      <c r="BJ3" s="2" t="n"/>
-      <c r="BK3" s="2" t="n"/>
-      <c r="BL3" s="2" t="n"/>
-      <c r="BM3" s="2" t="n"/>
-      <c r="BN3" s="2" t="n"/>
-      <c r="BO3" s="2" t="n"/>
-      <c r="BP3" s="2" t="n"/>
-      <c r="BQ3" s="2" t="n"/>
-      <c r="BR3" s="2" t="n"/>
-      <c r="BS3" s="2" t="n"/>
-      <c r="BT3" s="2" t="n"/>
-      <c r="BU3" s="2" t="n"/>
-      <c r="BV3" s="2" t="n"/>
-      <c r="BW3" s="2" t="n"/>
-      <c r="BX3" s="2" t="n"/>
-      <c r="BY3" s="2" t="n"/>
-      <c r="BZ3" s="2" t="n"/>
-      <c r="CA3" s="2" t="n"/>
-      <c r="CB3" s="2" t="n"/>
-      <c r="CC3" s="2" t="n"/>
-      <c r="CD3" s="2" t="n"/>
-      <c r="CE3" s="2" t="n"/>
-      <c r="CF3" s="2">
-        <f>SUM(B3:CE3)</f>
+      <c r="AQ3" s="2">
+        <f>SUM(B3:AP3)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
NB4, 10, 11 angepasst, funktioniert nun
</commit_message>
<xml_diff>
--- a/Einsatzplan.xlsx
+++ b/Einsatzplan.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ3"/>
+  <dimension ref="A1:CF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,6 +472,47 @@
     <col width="3" customWidth="1" min="41" max="41"/>
     <col width="3" customWidth="1" min="42" max="42"/>
     <col width="3" customWidth="1" min="43" max="43"/>
+    <col width="3" customWidth="1" min="44" max="44"/>
+    <col width="3" customWidth="1" min="45" max="45"/>
+    <col width="3" customWidth="1" min="46" max="46"/>
+    <col width="3" customWidth="1" min="47" max="47"/>
+    <col width="3" customWidth="1" min="48" max="48"/>
+    <col width="3" customWidth="1" min="49" max="49"/>
+    <col width="3" customWidth="1" min="50" max="50"/>
+    <col width="3" customWidth="1" min="51" max="51"/>
+    <col width="3" customWidth="1" min="52" max="52"/>
+    <col width="3" customWidth="1" min="53" max="53"/>
+    <col width="3" customWidth="1" min="54" max="54"/>
+    <col width="3" customWidth="1" min="55" max="55"/>
+    <col width="3" customWidth="1" min="56" max="56"/>
+    <col width="3" customWidth="1" min="57" max="57"/>
+    <col width="3" customWidth="1" min="58" max="58"/>
+    <col width="3" customWidth="1" min="59" max="59"/>
+    <col width="3" customWidth="1" min="60" max="60"/>
+    <col width="3" customWidth="1" min="61" max="61"/>
+    <col width="3" customWidth="1" min="62" max="62"/>
+    <col width="3" customWidth="1" min="63" max="63"/>
+    <col width="3" customWidth="1" min="64" max="64"/>
+    <col width="3" customWidth="1" min="65" max="65"/>
+    <col width="3" customWidth="1" min="66" max="66"/>
+    <col width="3" customWidth="1" min="67" max="67"/>
+    <col width="3" customWidth="1" min="68" max="68"/>
+    <col width="3" customWidth="1" min="69" max="69"/>
+    <col width="3" customWidth="1" min="70" max="70"/>
+    <col width="3" customWidth="1" min="71" max="71"/>
+    <col width="3" customWidth="1" min="72" max="72"/>
+    <col width="3" customWidth="1" min="73" max="73"/>
+    <col width="3" customWidth="1" min="74" max="74"/>
+    <col width="3" customWidth="1" min="75" max="75"/>
+    <col width="3" customWidth="1" min="76" max="76"/>
+    <col width="3" customWidth="1" min="77" max="77"/>
+    <col width="3" customWidth="1" min="78" max="78"/>
+    <col width="3" customWidth="1" min="79" max="79"/>
+    <col width="3" customWidth="1" min="80" max="80"/>
+    <col width="3" customWidth="1" min="81" max="81"/>
+    <col width="3" customWidth="1" min="82" max="82"/>
+    <col width="3" customWidth="1" min="83" max="83"/>
+    <col width="3" customWidth="1" min="84" max="84"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -687,13 +728,218 @@
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
+          <t>T2, 8:0</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 8:15</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 8:30</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 8:45</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 9:0</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 9:15</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 9:30</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 9:45</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 10:0</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 10:15</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 10:30</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 10:45</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 11:0</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 11:15</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 11:30</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 11:45</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 12:0</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 12:15</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 12:30</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 12:45</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 13:0</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 13:15</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 13:30</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 13:45</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 14:0</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 14:15</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 14:30</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 14:45</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 15:0</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 15:15</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 15:30</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 15:45</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 16:0</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 16:15</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 16:30</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 16:45</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 17:0</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 17:15</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 17:30</t>
+        </is>
+      </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 17:45</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
           <t>Total Hours</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
@@ -720,22 +966,86 @@
           <t> </t>
         </is>
       </c>
-      <c r="G2" s="2" t="n"/>
-      <c r="H2" s="2" t="n"/>
-      <c r="I2" s="2" t="n"/>
-      <c r="J2" s="2" t="n"/>
-      <c r="K2" s="2" t="n"/>
-      <c r="L2" s="2" t="n"/>
-      <c r="M2" s="2" t="n"/>
-      <c r="N2" s="2" t="n"/>
-      <c r="O2" s="2" t="n"/>
-      <c r="P2" s="2" t="n"/>
-      <c r="Q2" s="2" t="n"/>
-      <c r="R2" s="2" t="n"/>
-      <c r="S2" s="2" t="n"/>
-      <c r="T2" s="2" t="n"/>
-      <c r="U2" s="2" t="n"/>
-      <c r="V2" s="2" t="n"/>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="P2" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="Q2" s="2" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="R2" s="2" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="S2" s="2" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="T2" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="U2" s="2" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="V2" s="2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="W2" s="2" t="n"/>
       <c r="X2" s="2" t="n"/>
       <c r="Y2" s="2" t="n"/>
@@ -756,14 +1066,55 @@
       <c r="AN2" s="2" t="n"/>
       <c r="AO2" s="2" t="n"/>
       <c r="AP2" s="2" t="n"/>
-      <c r="AQ2" s="2">
-        <f>SUM(B2:AP2)</f>
+      <c r="AQ2" s="2" t="n"/>
+      <c r="AR2" s="2" t="n"/>
+      <c r="AS2" s="2" t="n"/>
+      <c r="AT2" s="2" t="n"/>
+      <c r="AU2" s="2" t="n"/>
+      <c r="AV2" s="2" t="n"/>
+      <c r="AW2" s="2" t="n"/>
+      <c r="AX2" s="2" t="n"/>
+      <c r="AY2" s="2" t="n"/>
+      <c r="AZ2" s="2" t="n"/>
+      <c r="BA2" s="2" t="n"/>
+      <c r="BB2" s="2" t="n"/>
+      <c r="BC2" s="2" t="n"/>
+      <c r="BD2" s="2" t="n"/>
+      <c r="BE2" s="2" t="n"/>
+      <c r="BF2" s="2" t="n"/>
+      <c r="BG2" s="2" t="n"/>
+      <c r="BH2" s="2" t="n"/>
+      <c r="BI2" s="2" t="n"/>
+      <c r="BJ2" s="2" t="n"/>
+      <c r="BK2" s="2" t="n"/>
+      <c r="BL2" s="2" t="n"/>
+      <c r="BM2" s="2" t="n"/>
+      <c r="BN2" s="2" t="n"/>
+      <c r="BO2" s="2" t="n"/>
+      <c r="BP2" s="2" t="n"/>
+      <c r="BQ2" s="2" t="n"/>
+      <c r="BR2" s="2" t="n"/>
+      <c r="BS2" s="2" t="n"/>
+      <c r="BT2" s="2" t="n"/>
+      <c r="BU2" s="2" t="n"/>
+      <c r="BV2" s="2" t="n"/>
+      <c r="BW2" s="2" t="n"/>
+      <c r="BX2" s="2" t="n"/>
+      <c r="BY2" s="2" t="n"/>
+      <c r="BZ2" s="2" t="n"/>
+      <c r="CA2" s="2" t="n"/>
+      <c r="CB2" s="2" t="n"/>
+      <c r="CC2" s="2" t="n"/>
+      <c r="CD2" s="2" t="n"/>
+      <c r="CE2" s="2" t="n"/>
+      <c r="CF2" s="2">
+        <f>SUM(B2:CE2)</f>
         <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
@@ -790,86 +1141,22 @@
           <t> </t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>v</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
-        <is>
-          <t>i</t>
-        </is>
-      </c>
-      <c r="L3" s="2" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="M3" s="2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="N3" s="2" t="inlineStr">
-        <is>
-          <t>p</t>
-        </is>
-      </c>
-      <c r="O3" s="2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="P3" s="2" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="Q3" s="2" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="R3" s="2" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="S3" s="2" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="T3" s="2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="U3" s="2" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-      <c r="V3" s="2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="G3" s="2" t="n"/>
+      <c r="H3" s="2" t="n"/>
+      <c r="I3" s="2" t="n"/>
+      <c r="J3" s="2" t="n"/>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="n"/>
+      <c r="O3" s="2" t="n"/>
+      <c r="P3" s="2" t="n"/>
+      <c r="Q3" s="2" t="n"/>
+      <c r="R3" s="2" t="n"/>
+      <c r="S3" s="2" t="n"/>
+      <c r="T3" s="2" t="n"/>
+      <c r="U3" s="2" t="n"/>
+      <c r="V3" s="2" t="n"/>
       <c r="W3" s="2" t="n"/>
       <c r="X3" s="2" t="n"/>
       <c r="Y3" s="2" t="n"/>
@@ -890,8 +1177,49 @@
       <c r="AN3" s="2" t="n"/>
       <c r="AO3" s="2" t="n"/>
       <c r="AP3" s="2" t="n"/>
-      <c r="AQ3" s="2">
-        <f>SUM(B3:AP3)</f>
+      <c r="AQ3" s="2" t="n"/>
+      <c r="AR3" s="2" t="n"/>
+      <c r="AS3" s="2" t="n"/>
+      <c r="AT3" s="2" t="n"/>
+      <c r="AU3" s="2" t="n"/>
+      <c r="AV3" s="2" t="n"/>
+      <c r="AW3" s="2" t="n"/>
+      <c r="AX3" s="2" t="n"/>
+      <c r="AY3" s="2" t="n"/>
+      <c r="AZ3" s="2" t="n"/>
+      <c r="BA3" s="2" t="n"/>
+      <c r="BB3" s="2" t="n"/>
+      <c r="BC3" s="2" t="n"/>
+      <c r="BD3" s="2" t="n"/>
+      <c r="BE3" s="2" t="n"/>
+      <c r="BF3" s="2" t="n"/>
+      <c r="BG3" s="2" t="n"/>
+      <c r="BH3" s="2" t="n"/>
+      <c r="BI3" s="2" t="n"/>
+      <c r="BJ3" s="2" t="n"/>
+      <c r="BK3" s="2" t="n"/>
+      <c r="BL3" s="2" t="n"/>
+      <c r="BM3" s="2" t="n"/>
+      <c r="BN3" s="2" t="n"/>
+      <c r="BO3" s="2" t="n"/>
+      <c r="BP3" s="2" t="n"/>
+      <c r="BQ3" s="2" t="n"/>
+      <c r="BR3" s="2" t="n"/>
+      <c r="BS3" s="2" t="n"/>
+      <c r="BT3" s="2" t="n"/>
+      <c r="BU3" s="2" t="n"/>
+      <c r="BV3" s="2" t="n"/>
+      <c r="BW3" s="2" t="n"/>
+      <c r="BX3" s="2" t="n"/>
+      <c r="BY3" s="2" t="n"/>
+      <c r="BZ3" s="2" t="n"/>
+      <c r="CA3" s="2" t="n"/>
+      <c r="CB3" s="2" t="n"/>
+      <c r="CC3" s="2" t="n"/>
+      <c r="CD3" s="2" t="n"/>
+      <c r="CE3" s="2" t="n"/>
+      <c r="CF3" s="2">
+        <f>SUM(B3:CE3)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Kleine anpassung in binaere_liste -> timedelta(0)
</commit_message>
<xml_diff>
--- a/Einsatzplan.xlsx
+++ b/Einsatzplan.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CF3"/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,47 +472,6 @@
     <col width="3" customWidth="1" min="41" max="41"/>
     <col width="3" customWidth="1" min="42" max="42"/>
     <col width="3" customWidth="1" min="43" max="43"/>
-    <col width="3" customWidth="1" min="44" max="44"/>
-    <col width="3" customWidth="1" min="45" max="45"/>
-    <col width="3" customWidth="1" min="46" max="46"/>
-    <col width="3" customWidth="1" min="47" max="47"/>
-    <col width="3" customWidth="1" min="48" max="48"/>
-    <col width="3" customWidth="1" min="49" max="49"/>
-    <col width="3" customWidth="1" min="50" max="50"/>
-    <col width="3" customWidth="1" min="51" max="51"/>
-    <col width="3" customWidth="1" min="52" max="52"/>
-    <col width="3" customWidth="1" min="53" max="53"/>
-    <col width="3" customWidth="1" min="54" max="54"/>
-    <col width="3" customWidth="1" min="55" max="55"/>
-    <col width="3" customWidth="1" min="56" max="56"/>
-    <col width="3" customWidth="1" min="57" max="57"/>
-    <col width="3" customWidth="1" min="58" max="58"/>
-    <col width="3" customWidth="1" min="59" max="59"/>
-    <col width="3" customWidth="1" min="60" max="60"/>
-    <col width="3" customWidth="1" min="61" max="61"/>
-    <col width="3" customWidth="1" min="62" max="62"/>
-    <col width="3" customWidth="1" min="63" max="63"/>
-    <col width="3" customWidth="1" min="64" max="64"/>
-    <col width="3" customWidth="1" min="65" max="65"/>
-    <col width="3" customWidth="1" min="66" max="66"/>
-    <col width="3" customWidth="1" min="67" max="67"/>
-    <col width="3" customWidth="1" min="68" max="68"/>
-    <col width="3" customWidth="1" min="69" max="69"/>
-    <col width="3" customWidth="1" min="70" max="70"/>
-    <col width="3" customWidth="1" min="71" max="71"/>
-    <col width="3" customWidth="1" min="72" max="72"/>
-    <col width="3" customWidth="1" min="73" max="73"/>
-    <col width="3" customWidth="1" min="74" max="74"/>
-    <col width="3" customWidth="1" min="75" max="75"/>
-    <col width="3" customWidth="1" min="76" max="76"/>
-    <col width="3" customWidth="1" min="77" max="77"/>
-    <col width="3" customWidth="1" min="78" max="78"/>
-    <col width="3" customWidth="1" min="79" max="79"/>
-    <col width="3" customWidth="1" min="80" max="80"/>
-    <col width="3" customWidth="1" min="81" max="81"/>
-    <col width="3" customWidth="1" min="82" max="82"/>
-    <col width="3" customWidth="1" min="83" max="83"/>
-    <col width="3" customWidth="1" min="84" max="84"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -728,218 +687,13 @@
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>T2, 8:0</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 8:15</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 8:30</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 8:45</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 9:0</t>
-        </is>
-      </c>
-      <c r="AV1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 9:15</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 9:30</t>
-        </is>
-      </c>
-      <c r="AX1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 9:45</t>
-        </is>
-      </c>
-      <c r="AY1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 10:0</t>
-        </is>
-      </c>
-      <c r="AZ1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 10:15</t>
-        </is>
-      </c>
-      <c r="BA1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 10:30</t>
-        </is>
-      </c>
-      <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 10:45</t>
-        </is>
-      </c>
-      <c r="BC1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 11:0</t>
-        </is>
-      </c>
-      <c r="BD1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 11:15</t>
-        </is>
-      </c>
-      <c r="BE1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 11:30</t>
-        </is>
-      </c>
-      <c r="BF1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 11:45</t>
-        </is>
-      </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 12:0</t>
-        </is>
-      </c>
-      <c r="BH1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 12:15</t>
-        </is>
-      </c>
-      <c r="BI1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 12:30</t>
-        </is>
-      </c>
-      <c r="BJ1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 12:45</t>
-        </is>
-      </c>
-      <c r="BK1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 13:0</t>
-        </is>
-      </c>
-      <c r="BL1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 13:15</t>
-        </is>
-      </c>
-      <c r="BM1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 13:30</t>
-        </is>
-      </c>
-      <c r="BN1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 13:45</t>
-        </is>
-      </c>
-      <c r="BO1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 14:0</t>
-        </is>
-      </c>
-      <c r="BP1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 14:15</t>
-        </is>
-      </c>
-      <c r="BQ1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 14:30</t>
-        </is>
-      </c>
-      <c r="BR1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 14:45</t>
-        </is>
-      </c>
-      <c r="BS1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 15:0</t>
-        </is>
-      </c>
-      <c r="BT1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 15:15</t>
-        </is>
-      </c>
-      <c r="BU1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 15:30</t>
-        </is>
-      </c>
-      <c r="BV1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 15:45</t>
-        </is>
-      </c>
-      <c r="BW1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 16:0</t>
-        </is>
-      </c>
-      <c r="BX1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 16:15</t>
-        </is>
-      </c>
-      <c r="BY1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 16:30</t>
-        </is>
-      </c>
-      <c r="BZ1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 16:45</t>
-        </is>
-      </c>
-      <c r="CA1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 17:0</t>
-        </is>
-      </c>
-      <c r="CB1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 17:15</t>
-        </is>
-      </c>
-      <c r="CC1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 17:30</t>
-        </is>
-      </c>
-      <c r="CD1" s="1" t="inlineStr">
-        <is>
-          <t>T2, 17:45</t>
-        </is>
-      </c>
-      <c r="CE1" s="1" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="CF1" s="1" t="inlineStr">
-        <is>
           <t>Total Hours</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
@@ -966,86 +720,22 @@
           <t> </t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>v</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>i</t>
-        </is>
-      </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
-        <is>
-          <t>p</t>
-        </is>
-      </c>
-      <c r="O2" s="2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="P2" s="2" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="Q2" s="2" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="R2" s="2" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="S2" s="2" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="T2" s="2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="U2" s="2" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-      <c r="V2" s="2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
+      <c r="M2" s="2" t="n"/>
+      <c r="N2" s="2" t="n"/>
+      <c r="O2" s="2" t="n"/>
+      <c r="P2" s="2" t="n"/>
+      <c r="Q2" s="2" t="n"/>
+      <c r="R2" s="2" t="n"/>
+      <c r="S2" s="2" t="n"/>
+      <c r="T2" s="2" t="n"/>
+      <c r="U2" s="2" t="n"/>
+      <c r="V2" s="2" t="n"/>
       <c r="W2" s="2" t="n"/>
       <c r="X2" s="2" t="n"/>
       <c r="Y2" s="2" t="n"/>
@@ -1066,55 +756,14 @@
       <c r="AN2" s="2" t="n"/>
       <c r="AO2" s="2" t="n"/>
       <c r="AP2" s="2" t="n"/>
-      <c r="AQ2" s="2" t="n"/>
-      <c r="AR2" s="2" t="n"/>
-      <c r="AS2" s="2" t="n"/>
-      <c r="AT2" s="2" t="n"/>
-      <c r="AU2" s="2" t="n"/>
-      <c r="AV2" s="2" t="n"/>
-      <c r="AW2" s="2" t="n"/>
-      <c r="AX2" s="2" t="n"/>
-      <c r="AY2" s="2" t="n"/>
-      <c r="AZ2" s="2" t="n"/>
-      <c r="BA2" s="2" t="n"/>
-      <c r="BB2" s="2" t="n"/>
-      <c r="BC2" s="2" t="n"/>
-      <c r="BD2" s="2" t="n"/>
-      <c r="BE2" s="2" t="n"/>
-      <c r="BF2" s="2" t="n"/>
-      <c r="BG2" s="2" t="n"/>
-      <c r="BH2" s="2" t="n"/>
-      <c r="BI2" s="2" t="n"/>
-      <c r="BJ2" s="2" t="n"/>
-      <c r="BK2" s="2" t="n"/>
-      <c r="BL2" s="2" t="n"/>
-      <c r="BM2" s="2" t="n"/>
-      <c r="BN2" s="2" t="n"/>
-      <c r="BO2" s="2" t="n"/>
-      <c r="BP2" s="2" t="n"/>
-      <c r="BQ2" s="2" t="n"/>
-      <c r="BR2" s="2" t="n"/>
-      <c r="BS2" s="2" t="n"/>
-      <c r="BT2" s="2" t="n"/>
-      <c r="BU2" s="2" t="n"/>
-      <c r="BV2" s="2" t="n"/>
-      <c r="BW2" s="2" t="n"/>
-      <c r="BX2" s="2" t="n"/>
-      <c r="BY2" s="2" t="n"/>
-      <c r="BZ2" s="2" t="n"/>
-      <c r="CA2" s="2" t="n"/>
-      <c r="CB2" s="2" t="n"/>
-      <c r="CC2" s="2" t="n"/>
-      <c r="CD2" s="2" t="n"/>
-      <c r="CE2" s="2" t="n"/>
-      <c r="CF2" s="2">
-        <f>SUM(B2:CE2)</f>
+      <c r="AQ2" s="2">
+        <f>SUM(B2:AP2)</f>
         <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
@@ -1141,22 +790,86 @@
           <t> </t>
         </is>
       </c>
-      <c r="G3" s="2" t="n"/>
-      <c r="H3" s="2" t="n"/>
-      <c r="I3" s="2" t="n"/>
-      <c r="J3" s="2" t="n"/>
-      <c r="K3" s="2" t="n"/>
-      <c r="L3" s="2" t="n"/>
-      <c r="M3" s="2" t="n"/>
-      <c r="N3" s="2" t="n"/>
-      <c r="O3" s="2" t="n"/>
-      <c r="P3" s="2" t="n"/>
-      <c r="Q3" s="2" t="n"/>
-      <c r="R3" s="2" t="n"/>
-      <c r="S3" s="2" t="n"/>
-      <c r="T3" s="2" t="n"/>
-      <c r="U3" s="2" t="n"/>
-      <c r="V3" s="2" t="n"/>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="O3" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="Q3" s="2" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="R3" s="2" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="S3" s="2" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="U3" s="2" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="W3" s="2" t="n"/>
       <c r="X3" s="2" t="n"/>
       <c r="Y3" s="2" t="n"/>
@@ -1177,49 +890,8 @@
       <c r="AN3" s="2" t="n"/>
       <c r="AO3" s="2" t="n"/>
       <c r="AP3" s="2" t="n"/>
-      <c r="AQ3" s="2" t="n"/>
-      <c r="AR3" s="2" t="n"/>
-      <c r="AS3" s="2" t="n"/>
-      <c r="AT3" s="2" t="n"/>
-      <c r="AU3" s="2" t="n"/>
-      <c r="AV3" s="2" t="n"/>
-      <c r="AW3" s="2" t="n"/>
-      <c r="AX3" s="2" t="n"/>
-      <c r="AY3" s="2" t="n"/>
-      <c r="AZ3" s="2" t="n"/>
-      <c r="BA3" s="2" t="n"/>
-      <c r="BB3" s="2" t="n"/>
-      <c r="BC3" s="2" t="n"/>
-      <c r="BD3" s="2" t="n"/>
-      <c r="BE3" s="2" t="n"/>
-      <c r="BF3" s="2" t="n"/>
-      <c r="BG3" s="2" t="n"/>
-      <c r="BH3" s="2" t="n"/>
-      <c r="BI3" s="2" t="n"/>
-      <c r="BJ3" s="2" t="n"/>
-      <c r="BK3" s="2" t="n"/>
-      <c r="BL3" s="2" t="n"/>
-      <c r="BM3" s="2" t="n"/>
-      <c r="BN3" s="2" t="n"/>
-      <c r="BO3" s="2" t="n"/>
-      <c r="BP3" s="2" t="n"/>
-      <c r="BQ3" s="2" t="n"/>
-      <c r="BR3" s="2" t="n"/>
-      <c r="BS3" s="2" t="n"/>
-      <c r="BT3" s="2" t="n"/>
-      <c r="BU3" s="2" t="n"/>
-      <c r="BV3" s="2" t="n"/>
-      <c r="BW3" s="2" t="n"/>
-      <c r="BX3" s="2" t="n"/>
-      <c r="BY3" s="2" t="n"/>
-      <c r="BZ3" s="2" t="n"/>
-      <c r="CA3" s="2" t="n"/>
-      <c r="CB3" s="2" t="n"/>
-      <c r="CC3" s="2" t="n"/>
-      <c r="CD3" s="2" t="n"/>
-      <c r="CE3" s="2" t="n"/>
-      <c r="CF3" s="2">
-        <f>SUM(B3:CE3)</f>
+      <c r="AQ3" s="2">
+        <f>SUM(B3:AP3)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
def binaere_liste(self) Methode angepasst
</commit_message>
<xml_diff>
--- a/Einsatzplan.xlsx
+++ b/Einsatzplan.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ3"/>
+  <dimension ref="A1:CF5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,6 +472,47 @@
     <col width="3" customWidth="1" min="41" max="41"/>
     <col width="3" customWidth="1" min="42" max="42"/>
     <col width="3" customWidth="1" min="43" max="43"/>
+    <col width="3" customWidth="1" min="44" max="44"/>
+    <col width="3" customWidth="1" min="45" max="45"/>
+    <col width="3" customWidth="1" min="46" max="46"/>
+    <col width="3" customWidth="1" min="47" max="47"/>
+    <col width="3" customWidth="1" min="48" max="48"/>
+    <col width="3" customWidth="1" min="49" max="49"/>
+    <col width="3" customWidth="1" min="50" max="50"/>
+    <col width="3" customWidth="1" min="51" max="51"/>
+    <col width="3" customWidth="1" min="52" max="52"/>
+    <col width="3" customWidth="1" min="53" max="53"/>
+    <col width="3" customWidth="1" min="54" max="54"/>
+    <col width="3" customWidth="1" min="55" max="55"/>
+    <col width="3" customWidth="1" min="56" max="56"/>
+    <col width="3" customWidth="1" min="57" max="57"/>
+    <col width="3" customWidth="1" min="58" max="58"/>
+    <col width="3" customWidth="1" min="59" max="59"/>
+    <col width="3" customWidth="1" min="60" max="60"/>
+    <col width="3" customWidth="1" min="61" max="61"/>
+    <col width="3" customWidth="1" min="62" max="62"/>
+    <col width="3" customWidth="1" min="63" max="63"/>
+    <col width="3" customWidth="1" min="64" max="64"/>
+    <col width="3" customWidth="1" min="65" max="65"/>
+    <col width="3" customWidth="1" min="66" max="66"/>
+    <col width="3" customWidth="1" min="67" max="67"/>
+    <col width="3" customWidth="1" min="68" max="68"/>
+    <col width="3" customWidth="1" min="69" max="69"/>
+    <col width="3" customWidth="1" min="70" max="70"/>
+    <col width="3" customWidth="1" min="71" max="71"/>
+    <col width="3" customWidth="1" min="72" max="72"/>
+    <col width="3" customWidth="1" min="73" max="73"/>
+    <col width="3" customWidth="1" min="74" max="74"/>
+    <col width="3" customWidth="1" min="75" max="75"/>
+    <col width="3" customWidth="1" min="76" max="76"/>
+    <col width="3" customWidth="1" min="77" max="77"/>
+    <col width="3" customWidth="1" min="78" max="78"/>
+    <col width="3" customWidth="1" min="79" max="79"/>
+    <col width="3" customWidth="1" min="80" max="80"/>
+    <col width="3" customWidth="1" min="81" max="81"/>
+    <col width="3" customWidth="1" min="82" max="82"/>
+    <col width="3" customWidth="1" min="83" max="83"/>
+    <col width="3" customWidth="1" min="84" max="84"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -687,13 +728,218 @@
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
+          <t>T2, 8:0</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 8:15</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 8:30</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 8:45</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 9:0</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 9:15</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 9:30</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 9:45</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 10:0</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 10:15</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 10:30</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 10:45</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 11:0</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 11:15</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 11:30</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 11:45</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 12:0</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 12:15</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 12:30</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 12:45</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 13:0</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 13:15</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 13:30</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 13:45</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 14:0</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 14:15</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 14:30</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 14:45</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 15:0</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 15:15</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 15:30</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 15:45</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 16:0</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 16:15</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 16:30</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 16:45</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 17:0</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 17:15</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 17:30</t>
+        </is>
+      </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>T2, 17:45</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
           <t>Total Hours</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
@@ -720,22 +966,86 @@
           <t> </t>
         </is>
       </c>
-      <c r="G2" s="2" t="n"/>
-      <c r="H2" s="2" t="n"/>
-      <c r="I2" s="2" t="n"/>
-      <c r="J2" s="2" t="n"/>
-      <c r="K2" s="2" t="n"/>
-      <c r="L2" s="2" t="n"/>
-      <c r="M2" s="2" t="n"/>
-      <c r="N2" s="2" t="n"/>
-      <c r="O2" s="2" t="n"/>
-      <c r="P2" s="2" t="n"/>
-      <c r="Q2" s="2" t="n"/>
-      <c r="R2" s="2" t="n"/>
-      <c r="S2" s="2" t="n"/>
-      <c r="T2" s="2" t="n"/>
-      <c r="U2" s="2" t="n"/>
-      <c r="V2" s="2" t="n"/>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="P2" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="Q2" s="2" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="R2" s="2" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="S2" s="2" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="T2" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="U2" s="2" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="V2" s="2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="W2" s="2" t="n"/>
       <c r="X2" s="2" t="n"/>
       <c r="Y2" s="2" t="n"/>
@@ -756,14 +1066,55 @@
       <c r="AN2" s="2" t="n"/>
       <c r="AO2" s="2" t="n"/>
       <c r="AP2" s="2" t="n"/>
-      <c r="AQ2" s="2">
-        <f>SUM(B2:AP2)</f>
+      <c r="AQ2" s="2" t="n"/>
+      <c r="AR2" s="2" t="n"/>
+      <c r="AS2" s="2" t="n"/>
+      <c r="AT2" s="2" t="n"/>
+      <c r="AU2" s="2" t="n"/>
+      <c r="AV2" s="2" t="n"/>
+      <c r="AW2" s="2" t="n"/>
+      <c r="AX2" s="2" t="n"/>
+      <c r="AY2" s="2" t="n"/>
+      <c r="AZ2" s="2" t="n"/>
+      <c r="BA2" s="2" t="n"/>
+      <c r="BB2" s="2" t="n"/>
+      <c r="BC2" s="2" t="n"/>
+      <c r="BD2" s="2" t="n"/>
+      <c r="BE2" s="2" t="n"/>
+      <c r="BF2" s="2" t="n"/>
+      <c r="BG2" s="2" t="n"/>
+      <c r="BH2" s="2" t="n"/>
+      <c r="BI2" s="2" t="n"/>
+      <c r="BJ2" s="2" t="n"/>
+      <c r="BK2" s="2" t="n"/>
+      <c r="BL2" s="2" t="n"/>
+      <c r="BM2" s="2" t="n"/>
+      <c r="BN2" s="2" t="n"/>
+      <c r="BO2" s="2" t="n"/>
+      <c r="BP2" s="2" t="n"/>
+      <c r="BQ2" s="2" t="n"/>
+      <c r="BR2" s="2" t="n"/>
+      <c r="BS2" s="2" t="n"/>
+      <c r="BT2" s="2" t="n"/>
+      <c r="BU2" s="2" t="n"/>
+      <c r="BV2" s="2" t="n"/>
+      <c r="BW2" s="2" t="n"/>
+      <c r="BX2" s="2" t="n"/>
+      <c r="BY2" s="2" t="n"/>
+      <c r="BZ2" s="2" t="n"/>
+      <c r="CA2" s="2" t="n"/>
+      <c r="CB2" s="2" t="n"/>
+      <c r="CC2" s="2" t="n"/>
+      <c r="CD2" s="2" t="n"/>
+      <c r="CE2" s="2" t="n"/>
+      <c r="CF2" s="2">
+        <f>SUM(B2:CE2)</f>
         <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
@@ -890,8 +1241,399 @@
       <c r="AN3" s="2" t="n"/>
       <c r="AO3" s="2" t="n"/>
       <c r="AP3" s="2" t="n"/>
-      <c r="AQ3" s="2">
-        <f>SUM(B3:AP3)</f>
+      <c r="AQ3" s="2" t="n"/>
+      <c r="AR3" s="2" t="n"/>
+      <c r="AS3" s="2" t="n"/>
+      <c r="AT3" s="2" t="n"/>
+      <c r="AU3" s="2" t="n"/>
+      <c r="AV3" s="2" t="n"/>
+      <c r="AW3" s="2" t="n"/>
+      <c r="AX3" s="2" t="n"/>
+      <c r="AY3" s="2" t="n"/>
+      <c r="AZ3" s="2" t="n"/>
+      <c r="BA3" s="2" t="n"/>
+      <c r="BB3" s="2" t="n"/>
+      <c r="BC3" s="2" t="n"/>
+      <c r="BD3" s="2" t="n"/>
+      <c r="BE3" s="2" t="n"/>
+      <c r="BF3" s="2" t="n"/>
+      <c r="BG3" s="2" t="n"/>
+      <c r="BH3" s="2" t="n"/>
+      <c r="BI3" s="2" t="n"/>
+      <c r="BJ3" s="2" t="n"/>
+      <c r="BK3" s="2" t="n"/>
+      <c r="BL3" s="2" t="n"/>
+      <c r="BM3" s="2" t="n"/>
+      <c r="BN3" s="2" t="n"/>
+      <c r="BO3" s="2" t="n"/>
+      <c r="BP3" s="2" t="n"/>
+      <c r="BQ3" s="2" t="n"/>
+      <c r="BR3" s="2" t="n"/>
+      <c r="BS3" s="2" t="n"/>
+      <c r="BT3" s="2" t="n"/>
+      <c r="BU3" s="2" t="n"/>
+      <c r="BV3" s="2" t="n"/>
+      <c r="BW3" s="2" t="n"/>
+      <c r="BX3" s="2" t="n"/>
+      <c r="BY3" s="2" t="n"/>
+      <c r="BZ3" s="2" t="n"/>
+      <c r="CA3" s="2" t="n"/>
+      <c r="CB3" s="2" t="n"/>
+      <c r="CC3" s="2" t="n"/>
+      <c r="CD3" s="2" t="n"/>
+      <c r="CE3" s="2" t="n"/>
+      <c r="CF3" s="2">
+        <f>SUM(B3:CE3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>131</v>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="M4" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="N4" s="2" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="O4" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="P4" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="Q4" s="2" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="R4" s="2" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="S4" s="2" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="T4" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="U4" s="2" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="V4" s="2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="W4" s="2" t="n"/>
+      <c r="X4" s="2" t="n"/>
+      <c r="Y4" s="2" t="n"/>
+      <c r="Z4" s="2" t="n"/>
+      <c r="AA4" s="2" t="n"/>
+      <c r="AB4" s="2" t="n"/>
+      <c r="AC4" s="2" t="n"/>
+      <c r="AD4" s="2" t="n"/>
+      <c r="AE4" s="2" t="n"/>
+      <c r="AF4" s="2" t="n"/>
+      <c r="AG4" s="2" t="n"/>
+      <c r="AH4" s="2" t="n"/>
+      <c r="AI4" s="2" t="n"/>
+      <c r="AJ4" s="2" t="n"/>
+      <c r="AK4" s="2" t="n"/>
+      <c r="AL4" s="2" t="n"/>
+      <c r="AM4" s="2" t="n"/>
+      <c r="AN4" s="2" t="n"/>
+      <c r="AO4" s="2" t="n"/>
+      <c r="AP4" s="2" t="n"/>
+      <c r="AQ4" s="2" t="n"/>
+      <c r="AR4" s="2" t="n"/>
+      <c r="AS4" s="2" t="n"/>
+      <c r="AT4" s="2" t="n"/>
+      <c r="AU4" s="2" t="n"/>
+      <c r="AV4" s="2" t="n"/>
+      <c r="AW4" s="2" t="n"/>
+      <c r="AX4" s="2" t="n"/>
+      <c r="AY4" s="2" t="n"/>
+      <c r="AZ4" s="2" t="n"/>
+      <c r="BA4" s="2" t="n"/>
+      <c r="BB4" s="2" t="n"/>
+      <c r="BC4" s="2" t="n"/>
+      <c r="BD4" s="2" t="n"/>
+      <c r="BE4" s="2" t="n"/>
+      <c r="BF4" s="2" t="n"/>
+      <c r="BG4" s="2" t="n"/>
+      <c r="BH4" s="2" t="n"/>
+      <c r="BI4" s="2" t="n"/>
+      <c r="BJ4" s="2" t="n"/>
+      <c r="BK4" s="2" t="n"/>
+      <c r="BL4" s="2" t="n"/>
+      <c r="BM4" s="2" t="n"/>
+      <c r="BN4" s="2" t="n"/>
+      <c r="BO4" s="2" t="n"/>
+      <c r="BP4" s="2" t="n"/>
+      <c r="BQ4" s="2" t="n"/>
+      <c r="BR4" s="2" t="n"/>
+      <c r="BS4" s="2" t="n"/>
+      <c r="BT4" s="2" t="n"/>
+      <c r="BU4" s="2" t="n"/>
+      <c r="BV4" s="2" t="n"/>
+      <c r="BW4" s="2" t="n"/>
+      <c r="BX4" s="2" t="n"/>
+      <c r="BY4" s="2" t="n"/>
+      <c r="BZ4" s="2" t="n"/>
+      <c r="CA4" s="2" t="n"/>
+      <c r="CB4" s="2" t="n"/>
+      <c r="CC4" s="2" t="n"/>
+      <c r="CD4" s="2" t="n"/>
+      <c r="CE4" s="2" t="n"/>
+      <c r="CF4" s="2">
+        <f>SUM(B4:CE4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>132</v>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="N5" s="2" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="O5" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="P5" s="2" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="Q5" s="2" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="R5" s="2" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="S5" s="2" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="T5" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="U5" s="2" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="V5" s="2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="W5" s="2" t="n"/>
+      <c r="X5" s="2" t="n"/>
+      <c r="Y5" s="2" t="n"/>
+      <c r="Z5" s="2" t="n"/>
+      <c r="AA5" s="2" t="n"/>
+      <c r="AB5" s="2" t="n"/>
+      <c r="AC5" s="2" t="n"/>
+      <c r="AD5" s="2" t="n"/>
+      <c r="AE5" s="2" t="n"/>
+      <c r="AF5" s="2" t="n"/>
+      <c r="AG5" s="2" t="n"/>
+      <c r="AH5" s="2" t="n"/>
+      <c r="AI5" s="2" t="n"/>
+      <c r="AJ5" s="2" t="n"/>
+      <c r="AK5" s="2" t="n"/>
+      <c r="AL5" s="2" t="n"/>
+      <c r="AM5" s="2" t="n"/>
+      <c r="AN5" s="2" t="n"/>
+      <c r="AO5" s="2" t="n"/>
+      <c r="AP5" s="2" t="n"/>
+      <c r="AQ5" s="2" t="n"/>
+      <c r="AR5" s="2" t="n"/>
+      <c r="AS5" s="2" t="n"/>
+      <c r="AT5" s="2" t="n"/>
+      <c r="AU5" s="2" t="n"/>
+      <c r="AV5" s="2" t="n"/>
+      <c r="AW5" s="2" t="n"/>
+      <c r="AX5" s="2" t="n"/>
+      <c r="AY5" s="2" t="n"/>
+      <c r="AZ5" s="2" t="n"/>
+      <c r="BA5" s="2" t="n"/>
+      <c r="BB5" s="2" t="n"/>
+      <c r="BC5" s="2" t="n"/>
+      <c r="BD5" s="2" t="n"/>
+      <c r="BE5" s="2" t="n"/>
+      <c r="BF5" s="2" t="n"/>
+      <c r="BG5" s="2" t="n"/>
+      <c r="BH5" s="2" t="n"/>
+      <c r="BI5" s="2" t="n"/>
+      <c r="BJ5" s="2" t="n"/>
+      <c r="BK5" s="2" t="n"/>
+      <c r="BL5" s="2" t="n"/>
+      <c r="BM5" s="2" t="n"/>
+      <c r="BN5" s="2" t="n"/>
+      <c r="BO5" s="2" t="n"/>
+      <c r="BP5" s="2" t="n"/>
+      <c r="BQ5" s="2" t="n"/>
+      <c r="BR5" s="2" t="n"/>
+      <c r="BS5" s="2" t="n"/>
+      <c r="BT5" s="2" t="n"/>
+      <c r="BU5" s="2" t="n"/>
+      <c r="BV5" s="2" t="n"/>
+      <c r="BW5" s="2" t="n"/>
+      <c r="BX5" s="2" t="n"/>
+      <c r="BY5" s="2" t="n"/>
+      <c r="BZ5" s="2" t="n"/>
+      <c r="CA5" s="2" t="n"/>
+      <c r="CB5" s="2" t="n"/>
+      <c r="CC5" s="2" t="n"/>
+      <c r="CD5" s="2" t="n"/>
+      <c r="CE5" s="2" t="n"/>
+      <c r="CF5" s="2">
+        <f>SUM(B5:CE5)</f>
         <v/>
       </c>
     </row>

</xml_diff>